<commit_message>
Update leaderboard - 2025-10-12 15:19:26
</commit_message>
<xml_diff>
--- a/docs/leaderboard.xlsx
+++ b/docs/leaderboard.xlsx
@@ -479,15 +479,15 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>리로 📈 ⭐
+          <t>리로
 @lee-lo-4u</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>549</v>
+        <v>659</v>
       </c>
       <c r="C2" t="n">
-        <v>407</v>
+        <v>519</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -496,205 +496,145 @@
         <v>128</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>김소윤
-@catmocotto</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>조한준
+@Desde_Seúl</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>255</v>
+      </c>
+      <c r="C3" t="n">
+        <v>161</v>
+      </c>
+      <c r="D3" t="n">
+        <v>76</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
+          <t>김소윤 🔥
+@catmocotto</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>임동한 🔥
+@easyfood369</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>김수정 🔥
+@kokonyang-p6l</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
           <t>강민성
 @IQ160건강깡패</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>김예림
 @vitaminute4u</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>조한준
-@Desde_Seúl</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>임동한
-@easyfood369</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>김수정
-@kokonyang-p6l</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>데이터 부족</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update leaderboard - 2025-10-13 03:41:11
</commit_message>
<xml_diff>
--- a/docs/leaderboard.xlsx
+++ b/docs/leaderboard.xlsx
@@ -484,19 +484,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>659</v>
+        <v>605</v>
       </c>
       <c r="C2" t="n">
-        <v>519</v>
+        <v>464</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>128</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Update leaderboard - 2025-10-13 13:37:46
</commit_message>
<xml_diff>
--- a/docs/leaderboard.xlsx
+++ b/docs/leaderboard.xlsx
@@ -484,19 +484,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>605</v>
+        <v>700</v>
       </c>
       <c r="C2" t="n">
-        <v>464</v>
+        <v>560</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>128</v>
       </c>
       <c r="F2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -507,16 +507,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C3" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D3" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>

</xml_diff>